<commit_message>
fin clase 3 in
</commit_message>
<xml_diff>
--- a/Archivos/ventas_excel.xlsx
+++ b/Archivos/ventas_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,16 @@
           <t>Descuentos</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Aportes</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Turno</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -465,6 +475,14 @@
       <c r="D2" t="n">
         <v>0.1</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.1139778962782939</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Nocturno</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -481,6 +499,14 @@
       <c r="D3" t="n">
         <v>0.2</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.04743262275842433</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Nocturno</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -497,6 +523,14 @@
       <c r="D4" t="n">
         <v>0.5</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.1976395354900047</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Diurno</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -513,6 +547,14 @@
       <c r="D5" t="n">
         <v>0.6</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1655148352056989</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Nocturno</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -529,6 +571,14 @@
       <c r="D6" t="n">
         <v>0.8</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.1026941048696355</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Nocturno</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -545,6 +595,14 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.05807755618836215</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Diurno</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -561,6 +619,14 @@
       <c r="D8" t="n">
         <v>0.3</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.156111127963929</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Diurno</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -577,6 +643,14 @@
       <c r="D9" t="n">
         <v>0.2</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.07690169178220757</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Diurno</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -593,6 +667,14 @@
       <c r="D10" t="n">
         <v>0.1</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.1674846750856551</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Nocturno</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -608,6 +690,14 @@
       </c>
       <c r="D11" t="n">
         <v>0.1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0372984697196711</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Diurno</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>